<commit_message>
Roger's Updates from Sat 12-7 Meeting
</commit_message>
<xml_diff>
--- a/ProjectDoc/GP Genie Traceability Matrix.xlsx
+++ b/ProjectDoc/GP Genie Traceability Matrix.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Susan\Documents\GitHub\GPGenie\ProjectDoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roger Peterson\Documents\GitHub\GPGenie\ProjectDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="948" yWindow="0" windowWidth="22092" windowHeight="9960"/>
+    <workbookView xWindow="75" yWindow="-30" windowWidth="14805" windowHeight="14325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="99">
   <si>
     <t>Project:</t>
   </si>
@@ -97,12 +97,6 @@
     <t>Req. #</t>
   </si>
   <si>
-    <t>REQUIREMENT DESCRIPTION  -  SRS SPECIFICATION # XXXXXX</t>
-  </si>
-  <si>
-    <t>TEST CASE  VER  XXXXXX SECTION(S)</t>
-  </si>
-  <si>
     <t>DOC. NO./  REPORT(S)</t>
   </si>
   <si>
@@ -112,21 +106,12 @@
     <t>Program shall obtain initial input configuration value from the user for population size.</t>
   </si>
   <si>
-    <t>X.X, X.X.X</t>
-  </si>
-  <si>
-    <t>XXXXXX-P, XXXXXX-R</t>
-  </si>
-  <si>
     <t>REQ-2</t>
   </si>
   <si>
     <t>Program shall obtain initial input configuration value from the user for maximum tree depth</t>
   </si>
   <si>
-    <t>Memo to leverage from XXXXXX-R</t>
-  </si>
-  <si>
     <t>REQ-3</t>
   </si>
   <si>
@@ -235,9 +220,6 @@
     <t>REQ-20</t>
   </si>
   <si>
-    <t>Program shall pair the postselection population individuals randomly creating pairs of parents.</t>
-  </si>
-  <si>
     <t>REQ-21</t>
   </si>
   <si>
@@ -269,13 +251,127 @@
   </si>
   <si>
     <t>Stretch: Program shall evaluate the fitness, to match equation Y = (-3X^3 + 7) / 2), of each individual in each population using training data -2 &lt;= X &lt;= 2.</t>
+  </si>
+  <si>
+    <t>Type of Test</t>
+  </si>
+  <si>
+    <t>Positive and Negative Test Script</t>
+  </si>
+  <si>
+    <t>TC.01 / TC.02</t>
+  </si>
+  <si>
+    <t>TC.03 / TC.04</t>
+  </si>
+  <si>
+    <t>Verification</t>
+  </si>
+  <si>
+    <t>TC.09</t>
+  </si>
+  <si>
+    <t>TC.11 / TC.12</t>
+  </si>
+  <si>
+    <t>TC.09 / TC.10</t>
+  </si>
+  <si>
+    <t>TEST CASE  VER  01    SECTION(S)</t>
+  </si>
+  <si>
+    <t>TC.05 / TC.06</t>
+  </si>
+  <si>
+    <t>TC.07 / TC.08</t>
+  </si>
+  <si>
+    <t>Unit Test Script</t>
+  </si>
+  <si>
+    <t>REQ-8.1</t>
+  </si>
+  <si>
+    <t>TC.19 / TC.20</t>
+  </si>
+  <si>
+    <t>TC.12</t>
+  </si>
+  <si>
+    <t>Code Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC.13 </t>
+  </si>
+  <si>
+    <t>TC.14</t>
+  </si>
+  <si>
+    <t>TC.15</t>
+  </si>
+  <si>
+    <t>TC.16</t>
+  </si>
+  <si>
+    <t>TC.17</t>
+  </si>
+  <si>
+    <t>TC.24 / TC.25</t>
+  </si>
+  <si>
+    <t>TC.18</t>
+  </si>
+  <si>
+    <t>TC.21</t>
+  </si>
+  <si>
+    <t>TC.22</t>
+  </si>
+  <si>
+    <t>TC.23</t>
+  </si>
+  <si>
+    <t>TC.26</t>
+  </si>
+  <si>
+    <t>TC.27</t>
+  </si>
+  <si>
+    <t>TC.28</t>
+  </si>
+  <si>
+    <t>TC.29</t>
+  </si>
+  <si>
+    <t>Verification                      (Unit Test Script)</t>
+  </si>
+  <si>
+    <t>REQUIREMENT DESCRIPTION  -  SRS SPECIFICATION Ver 1 Draft B</t>
+  </si>
+  <si>
+    <t>TC.30</t>
+  </si>
+  <si>
+    <t>Code Review (Negative test case design)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code Review / Test Script </t>
+  </si>
+  <si>
+    <t>Program shall pair the post selection population individuals randomly creating pairs of parents.</t>
+  </si>
+  <si>
+    <t>Code Review / User Test</t>
+  </si>
+  <si>
+    <t>TC.31 / TC.32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -304,11 +400,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
@@ -463,6 +554,25 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -791,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -804,106 +914,151 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,7 +1089,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -952,6 +1107,54 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7953375"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
@@ -1013,7 +1216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1048,7 +1251,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1233,899 +1436,1007 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="14" customWidth="1"/>
-    <col min="3" max="3" width="71.5546875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="5" style="22" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="71.5703125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
-      <c r="B1" s="22"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="7"/>
       <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="26"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="41"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
-      <c r="B2" s="22"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="7"/>
       <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="27"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="42"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="22"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="7"/>
       <c r="D3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="27"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="F3" s="42"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="13"/>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="42"/>
+    </row>
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+    </row>
+    <row r="6" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="47"/>
+      <c r="F7" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="34">
+        <v>1</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="27"/>
-    </row>
-    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="E8" s="40"/>
+      <c r="F8" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="34">
+        <v>2</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="40"/>
+      <c r="F9" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="34">
+        <v>3</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="34">
+        <v>4</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34">
+        <v>5</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="34">
         <v>6</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-    </row>
-    <row r="6" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="B13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="34">
         <v>7</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B14" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="34">
         <v>8</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="B15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="34">
         <v>9</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="B16" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34">
         <v>10</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="5" t="s">
+      <c r="B17" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="34">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
-        <v>1</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="B18" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="40"/>
+      <c r="F18" s="32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="34">
         <v>12</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="B19" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="40"/>
+      <c r="F19" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="34">
         <v>13</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="B20" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="34">
         <v>14</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="1" t="s">
+      <c r="B21" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="40"/>
+      <c r="F21" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="34">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
-        <v>2</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="B22" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="40"/>
+      <c r="F22" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="34">
+        <v>15</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="34">
         <v>17</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="1" t="s">
+      <c r="B24" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="40"/>
+      <c r="F24" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="34">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
-        <v>3</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="B25" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="40"/>
+      <c r="F25" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="34">
         <v>19</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="B26" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="40"/>
+      <c r="F26" s="32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="24"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+    </row>
+    <row r="29" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+    </row>
+    <row r="30" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="23" t="str">
+        <f>C7</f>
+        <v>REQUIREMENT DESCRIPTION  -  SRS SPECIFICATION Ver 1 Draft B</v>
+      </c>
+      <c r="D30" s="49" t="str">
+        <f>D7</f>
+        <v>TEST CASE  VER  01    SECTION(S)</v>
+      </c>
+      <c r="E30" s="47"/>
+      <c r="F30" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="34">
         <v>20</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
-        <v>4</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="B31" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="51"/>
+      <c r="F31" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="34">
         <v>21</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="B32" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="51"/>
+      <c r="F32" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="34">
         <v>22</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
-        <v>5</v>
-      </c>
-      <c r="B12" s="12" t="s">
+      <c r="B33" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="51"/>
+      <c r="F33" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="34">
         <v>23</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="B34" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="51"/>
+      <c r="F34" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="34">
         <v>24</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
-        <v>6</v>
-      </c>
-      <c r="B13" s="12" t="s">
+      <c r="B35" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="51"/>
+      <c r="F35" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="34">
         <v>25</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="B36" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="51"/>
+      <c r="F36" s="35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="34">
         <v>26</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="B37" s="26"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="34">
+        <v>27</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="34">
+        <v>28</v>
+      </c>
+      <c r="B39" s="26"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="34">
+        <v>29</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="34">
+        <v>30</v>
+      </c>
+      <c r="B41" s="26"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="34">
+        <v>31</v>
+      </c>
+      <c r="B42" s="26"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="34">
+        <v>32</v>
+      </c>
+      <c r="B43" s="26"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="34">
+        <v>33</v>
+      </c>
+      <c r="B44" s="26"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="34">
+        <v>34</v>
+      </c>
+      <c r="B45" s="26"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="34">
+        <v>35</v>
+      </c>
+      <c r="B46" s="26"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="34">
+        <v>36</v>
+      </c>
+      <c r="B47" s="26"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="34">
+        <v>37</v>
+      </c>
+      <c r="B48" s="26"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="34">
+        <v>38</v>
+      </c>
+      <c r="B49" s="26"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="24"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+    </row>
+    <row r="52" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="20"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+    </row>
+    <row r="53" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
-        <v>8</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="B53" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="23" t="str">
+        <f>C7</f>
+        <v>REQUIREMENT DESCRIPTION  -  SRS SPECIFICATION Ver 1 Draft B</v>
+      </c>
+      <c r="D53" s="49" t="str">
+        <f>D7</f>
+        <v>TEST CASE  VER  01    SECTION(S)</v>
+      </c>
+      <c r="E53" s="47"/>
+      <c r="F53" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
-        <v>10</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
-        <v>11</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
-        <v>12</v>
-      </c>
-      <c r="B19" s="12" t="s">
+    </row>
+    <row r="54" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="19">
         <v>37</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
-        <v>13</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
-        <v>14</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
-        <v>15</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
-        <v>16</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="32"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
-        <v>16</v>
-      </c>
-      <c r="B24" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
-        <v>17</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-    </row>
-    <row r="28" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="24" t="str">
-        <f>C7</f>
-        <v>REQUIREMENT DESCRIPTION  -  SRS SPECIFICATION # XXXXXX</v>
-      </c>
-      <c r="D29" s="30" t="str">
-        <f>D7</f>
-        <v>TEST CASE  VER  XXXXXX SECTION(S)</v>
-      </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20">
-        <v>18</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="19"/>
-    </row>
-    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20">
-        <v>19</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20">
-        <v>20</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
-        <v>21</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20">
-        <v>22</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20">
-        <v>23</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20">
-        <v>24</v>
-      </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20">
-        <v>25</v>
-      </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="20">
-        <v>26</v>
-      </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20">
-        <v>27</v>
-      </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20">
-        <v>28</v>
-      </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20">
-        <v>29</v>
-      </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20">
-        <v>30</v>
-      </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20">
-        <v>31</v>
-      </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20">
-        <v>32</v>
-      </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20">
-        <v>33</v>
-      </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20">
-        <v>34</v>
-      </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20">
-        <v>35</v>
-      </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20">
-        <v>36</v>
-      </c>
-      <c r="B48" s="12"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-    </row>
-    <row r="51" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-    </row>
-    <row r="52" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="24" t="str">
-        <f>C7</f>
-        <v>REQUIREMENT DESCRIPTION  -  SRS SPECIFICATION # XXXXXX</v>
-      </c>
-      <c r="D52" s="30" t="str">
-        <f>D7</f>
-        <v>TEST CASE  VER  XXXXXX SECTION(S)</v>
-      </c>
-      <c r="E52" s="31"/>
-      <c r="F52" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="20">
-        <v>37</v>
-      </c>
-      <c r="B53" s="12"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="19"/>
-    </row>
-    <row r="54" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="20">
-        <v>38</v>
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="11"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="20">
-        <v>39</v>
+      <c r="D54" s="52"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="18"/>
+    </row>
+    <row r="55" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="19">
+        <v>38</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="11"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="35"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="53"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
+    <row r="56" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="19">
+        <v>39</v>
+      </c>
       <c r="B56" s="12"/>
       <c r="C56" s="11"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="35"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="53"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
+    <row r="57" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="19"/>
       <c r="B57" s="12"/>
       <c r="C57" s="11"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="35"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="53"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
+    <row r="58" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="19"/>
       <c r="B58" s="12"/>
       <c r="C58" s="11"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="35"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="53"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
+    <row r="59" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="19"/>
       <c r="B59" s="12"/>
       <c r="C59" s="11"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="35"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="53"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
+    <row r="60" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="19"/>
       <c r="B60" s="12"/>
       <c r="C60" s="11"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="35"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="53"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
+    <row r="61" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="19"/>
       <c r="B61" s="12"/>
       <c r="C61" s="11"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="35"/>
+      <c r="D61" s="52"/>
+      <c r="E61" s="53"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
+    <row r="62" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="19"/>
       <c r="B62" s="12"/>
       <c r="C62" s="11"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="35"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="53"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
+    <row r="63" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="19"/>
       <c r="B63" s="12"/>
       <c r="C63" s="11"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="35"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="53"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
+    <row r="64" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="19"/>
       <c r="B64" s="12"/>
       <c r="C64" s="11"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="35"/>
+      <c r="D64" s="52"/>
+      <c r="E64" s="53"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
+    <row r="65" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="19"/>
       <c r="B65" s="12"/>
       <c r="C65" s="11"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="35"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="53"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
+    <row r="66" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="19"/>
       <c r="B66" s="12"/>
       <c r="C66" s="11"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="35"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="53"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
+    <row r="67" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="19"/>
       <c r="B67" s="12"/>
       <c r="C67" s="11"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="35"/>
+      <c r="D67" s="52"/>
+      <c r="E67" s="53"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
+    <row r="68" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="19"/>
       <c r="B68" s="12"/>
       <c r="C68" s="11"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="35"/>
+      <c r="D68" s="52"/>
+      <c r="E68" s="53"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
+    <row r="69" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="19"/>
       <c r="B69" s="12"/>
       <c r="C69" s="11"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="35"/>
+      <c r="D69" s="52"/>
+      <c r="E69" s="53"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
+    <row r="70" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="19"/>
       <c r="B70" s="12"/>
       <c r="C70" s="11"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="35"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="53"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="34"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="15"/>
+    <row r="71" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="19"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="52"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="4"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="52"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="67">
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D66:E66"/>
+  <mergeCells count="68">
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="D67:E67"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D71:E71"/>
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="D63:E63"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D66:E66"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A51:F51"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D56:E56"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D49:E49"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D44:E44"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D39:E39"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A28:F28"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2135,9 +2446,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2145,7 +2456,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2153,7 +2464,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -2161,7 +2472,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -2169,7 +2480,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2177,7 +2488,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2185,7 +2496,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2193,7 +2504,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2201,7 +2512,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2209,7 +2520,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2217,7 +2528,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2225,7 +2536,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2233,7 +2544,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -2241,7 +2552,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -2249,7 +2560,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -2257,7 +2568,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -2265,7 +2576,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -2273,7 +2584,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2281,7 +2592,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -2289,7 +2600,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2308,9 +2619,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2318,7 +2629,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2326,7 +2637,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -2334,7 +2645,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -2342,7 +2653,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2350,7 +2661,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2358,7 +2669,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2366,7 +2677,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2374,7 +2685,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2382,7 +2693,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2390,7 +2701,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2398,7 +2709,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2406,7 +2717,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -2414,7 +2725,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -2422,7 +2733,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -2430,7 +2741,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -2438,7 +2749,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -2446,7 +2757,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2454,7 +2765,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -2462,7 +2773,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>

</xml_diff>